<commit_message>
Novas sprites e logicas
</commit_message>
<xml_diff>
--- a/calc/matriz-gameboard-calc.xlsx
+++ b/calc/matriz-gameboard-calc.xlsx
@@ -407,7 +407,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -418,83 +418,125 @@
     <row r="1" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="C1" s="5">
         <f>B1+48</f>
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="D1" s="5">
         <f>C1+48</f>
-        <v>142</v>
+        <v>180</v>
       </c>
       <c r="E1" s="5">
         <f>D1+48</f>
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="F1" s="5">
-        <f t="shared" ref="E1:N1" si="0">E1+48</f>
-        <v>238</v>
+        <f t="shared" ref="F1:N1" si="0">E1+48</f>
+        <v>276</v>
       </c>
       <c r="G1" s="5">
         <f t="shared" si="0"/>
-        <v>286</v>
+        <v>324</v>
       </c>
       <c r="H1" s="5">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>372</v>
       </c>
       <c r="I1" s="5">
         <f t="shared" si="0"/>
-        <v>382</v>
+        <v>420</v>
       </c>
       <c r="J1" s="5">
         <f t="shared" si="0"/>
-        <v>430</v>
+        <v>468</v>
       </c>
       <c r="K1" s="5">
         <f t="shared" si="0"/>
-        <v>478</v>
+        <v>516</v>
       </c>
       <c r="L1" s="5">
         <f t="shared" si="0"/>
-        <v>526</v>
+        <v>564</v>
       </c>
       <c r="M1" s="5">
         <f t="shared" si="0"/>
-        <v>574</v>
+        <v>612</v>
       </c>
       <c r="N1" s="5">
         <f t="shared" si="0"/>
-        <v>622</v>
+        <v>660</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="B2" s="2">
+        <f>(B1-46)/48</f>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C2" s="3">
+        <f>(C1-46)/48</f>
+        <v>1.7916666666666667</v>
+      </c>
+      <c r="D2" s="2">
+        <f t="shared" ref="D2:N2" si="1">(D1-46)/48</f>
+        <v>2.7916666666666665</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" si="1"/>
+        <v>3.7916666666666665</v>
+      </c>
+      <c r="F2" s="2">
+        <f t="shared" si="1"/>
+        <v>4.791666666666667</v>
+      </c>
+      <c r="G2" s="3">
+        <f t="shared" si="1"/>
+        <v>5.791666666666667</v>
+      </c>
+      <c r="H2" s="2">
+        <f t="shared" si="1"/>
+        <v>6.791666666666667</v>
+      </c>
+      <c r="I2" s="3">
+        <f t="shared" si="1"/>
+        <v>7.791666666666667</v>
+      </c>
+      <c r="J2" s="2">
+        <f t="shared" si="1"/>
+        <v>8.7916666666666661</v>
+      </c>
+      <c r="K2" s="3">
+        <f t="shared" si="1"/>
+        <v>9.7916666666666661</v>
+      </c>
+      <c r="L2" s="3">
+        <f t="shared" si="1"/>
+        <v>10.791666666666666</v>
+      </c>
+      <c r="M2" s="3">
+        <f t="shared" si="1"/>
+        <v>11.791666666666666</v>
+      </c>
+      <c r="N2" s="2">
+        <f t="shared" si="1"/>
+        <v>12.791666666666666</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <f>A2+48</f>
-        <v>69</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>87</v>
+      </c>
+      <c r="B3" s="2">
+        <f>(A3-21)/48</f>
+        <v>1.375</v>
+      </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -508,10 +550,13 @@
     </row>
     <row r="4" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A10" si="1">A3+48</f>
-        <v>117</v>
-      </c>
-      <c r="B4" s="4"/>
+        <f t="shared" ref="A4:A10" si="2">A3+48</f>
+        <v>135</v>
+      </c>
+      <c r="B4" s="4">
+        <f t="shared" ref="B4:B10" si="3">(A4-21)/48</f>
+        <v>2.375</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2"/>
       <c r="E4" s="3"/>
@@ -527,15 +572,18 @@
     </row>
     <row r="5" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <f t="shared" si="1"/>
-        <v>165</v>
-      </c>
-      <c r="B5" s="2"/>
+        <f t="shared" si="2"/>
+        <v>183</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="3"/>
+        <v>3.375</v>
+      </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -546,10 +594,13 @@
     </row>
     <row r="6" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <f t="shared" si="1"/>
-        <v>213</v>
-      </c>
-      <c r="B6" s="3"/>
+        <f t="shared" si="2"/>
+        <v>231</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="3"/>
+        <v>4.375</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
@@ -565,14 +616,17 @@
     </row>
     <row r="7" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <f t="shared" si="1"/>
-        <v>261</v>
-      </c>
-      <c r="B7" s="3"/>
+        <f t="shared" si="2"/>
+        <v>279</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="3"/>
+        <v>5.375</v>
+      </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -584,10 +638,13 @@
     </row>
     <row r="8" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f t="shared" si="1"/>
-        <v>309</v>
-      </c>
-      <c r="B8" s="3"/>
+        <f t="shared" si="2"/>
+        <v>327</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="3"/>
+        <v>6.375</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
@@ -603,10 +660,13 @@
     </row>
     <row r="9" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f t="shared" si="1"/>
-        <v>357</v>
-      </c>
-      <c r="B9" s="3"/>
+        <f t="shared" si="2"/>
+        <v>375</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="3"/>
+        <v>7.375</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -622,10 +682,13 @@
     </row>
     <row r="10" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <f t="shared" si="1"/>
-        <v>405</v>
-      </c>
-      <c r="B10" s="3"/>
+        <f t="shared" si="2"/>
+        <v>423</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="3"/>
+        <v>8.375</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>

</xml_diff>

<commit_message>
Lógica explosão da bomba
</commit_message>
<xml_diff>
--- a/calc/matriz-gameboard-calc.xlsx
+++ b/calc/matriz-gameboard-calc.xlsx
@@ -33,18 +33,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -55,6 +49,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -91,16 +97,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -404,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -415,292 +421,360 @@
     <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5">
+    <row r="1" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3">
         <v>84</v>
       </c>
-      <c r="C1" s="5">
-        <f>B1+48</f>
-        <v>132</v>
-      </c>
-      <c r="D1" s="5">
-        <f>C1+48</f>
-        <v>180</v>
-      </c>
-      <c r="E1" s="5">
-        <f>D1+48</f>
-        <v>228</v>
-      </c>
-      <c r="F1" s="5">
-        <f t="shared" ref="F1:N1" si="0">E1+48</f>
-        <v>276</v>
-      </c>
-      <c r="G1" s="5">
-        <f t="shared" si="0"/>
-        <v>324</v>
-      </c>
-      <c r="H1" s="5">
-        <f t="shared" si="0"/>
-        <v>372</v>
-      </c>
-      <c r="I1" s="5">
+      <c r="C1" s="3">
+        <f>B1+42</f>
+        <v>126</v>
+      </c>
+      <c r="D1" s="3">
+        <f t="shared" ref="D1:N1" si="0">C1+42</f>
+        <v>168</v>
+      </c>
+      <c r="E1" s="3">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="F1" s="3">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="G1" s="3">
+        <f t="shared" si="0"/>
+        <v>294</v>
+      </c>
+      <c r="H1" s="3">
+        <f t="shared" si="0"/>
+        <v>336</v>
+      </c>
+      <c r="I1" s="3">
+        <f t="shared" si="0"/>
+        <v>378</v>
+      </c>
+      <c r="J1" s="3">
         <f t="shared" si="0"/>
         <v>420</v>
       </c>
-      <c r="J1" s="5">
-        <f t="shared" si="0"/>
-        <v>468</v>
-      </c>
-      <c r="K1" s="5">
-        <f t="shared" si="0"/>
-        <v>516</v>
-      </c>
-      <c r="L1" s="5">
-        <f t="shared" si="0"/>
-        <v>564</v>
-      </c>
-      <c r="M1" s="5">
-        <f t="shared" si="0"/>
-        <v>612</v>
-      </c>
-      <c r="N1" s="5">
-        <f t="shared" si="0"/>
-        <v>660</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2">
-        <f>(B1-46)/48</f>
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="C2" s="3">
-        <f>(C1-46)/48</f>
-        <v>1.7916666666666667</v>
-      </c>
-      <c r="D2" s="2">
-        <f t="shared" ref="D2:N2" si="1">(D1-46)/48</f>
-        <v>2.7916666666666665</v>
-      </c>
-      <c r="E2" s="3">
-        <f t="shared" si="1"/>
-        <v>3.7916666666666665</v>
-      </c>
-      <c r="F2" s="2">
-        <f t="shared" si="1"/>
-        <v>4.791666666666667</v>
-      </c>
-      <c r="G2" s="3">
-        <f t="shared" si="1"/>
-        <v>5.791666666666667</v>
-      </c>
-      <c r="H2" s="2">
-        <f t="shared" si="1"/>
-        <v>6.791666666666667</v>
-      </c>
-      <c r="I2" s="3">
-        <f t="shared" si="1"/>
-        <v>7.791666666666667</v>
-      </c>
-      <c r="J2" s="2">
-        <f t="shared" si="1"/>
-        <v>8.7916666666666661</v>
-      </c>
-      <c r="K2" s="3">
-        <f t="shared" si="1"/>
-        <v>9.7916666666666661</v>
-      </c>
-      <c r="L2" s="3">
-        <f t="shared" si="1"/>
-        <v>10.791666666666666</v>
-      </c>
-      <c r="M2" s="3">
-        <f t="shared" si="1"/>
-        <v>11.791666666666666</v>
-      </c>
-      <c r="N2" s="2">
-        <f t="shared" si="1"/>
-        <v>12.791666666666666</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <f>A2+48</f>
-        <v>87</v>
-      </c>
-      <c r="B3" s="2">
-        <f>(A3-21)/48</f>
-        <v>1.375</v>
-      </c>
-      <c r="C3" s="4"/>
+      <c r="K1" s="3">
+        <f t="shared" si="0"/>
+        <v>462</v>
+      </c>
+      <c r="L1" s="3">
+        <f t="shared" si="0"/>
+        <v>504</v>
+      </c>
+      <c r="M1" s="3">
+        <f t="shared" si="0"/>
+        <v>546</v>
+      </c>
+      <c r="N1" s="3">
+        <f t="shared" si="0"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>40</v>
+      </c>
+      <c r="B2" s="4">
+        <f>(B1-84)/42</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <f>(C1-84)/42</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <f t="shared" ref="C2:N2" si="1">(D1-84)/42</f>
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F2" s="4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G2" s="4">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H2" s="5">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I2" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J2" s="4">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K2" s="4">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="L2" s="4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M2" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="N2" s="4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <f>A2+42</f>
+        <v>82</v>
+      </c>
+      <c r="B3" s="4">
+        <f>(A3-39)/42</f>
+        <v>1.0238095238095237</v>
+      </c>
+      <c r="C3" s="5"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <f t="shared" ref="A4:A10" si="2">A3+48</f>
-        <v>135</v>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="4"/>
+      <c r="Q3" s="1">
+        <v>81</v>
+      </c>
+      <c r="R3" s="1">
+        <f>Q3-84</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A12" si="2">A3+42</f>
+        <v>124</v>
       </c>
       <c r="B4" s="4">
-        <f t="shared" ref="B4:B10" si="3">(A4-21)/48</f>
-        <v>2.375</v>
-      </c>
-      <c r="C4" s="3"/>
+        <f t="shared" ref="B4:B12" si="3">(A4-39)/42</f>
+        <v>2.0238095238095237</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="Q4" s="1">
+        <v>33</v>
+      </c>
+      <c r="R4" s="1">
+        <f>Q4-8</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <f t="shared" si="2"/>
-        <v>183</v>
-      </c>
-      <c r="B5" s="2">
+        <v>166</v>
+      </c>
+      <c r="B5" s="4">
         <f t="shared" si="3"/>
-        <v>3.375</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>3.0238095238095237</v>
+      </c>
+      <c r="C5" s="5"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <f t="shared" si="2"/>
-        <v>231</v>
-      </c>
-      <c r="B6" s="3">
+        <v>208</v>
+      </c>
+      <c r="B6" s="4">
         <f t="shared" si="3"/>
-        <v>4.375</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+        <v>4.0238095238095237</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="Q6" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <f t="shared" si="2"/>
-        <v>279</v>
-      </c>
-      <c r="B7" s="3">
+        <v>250</v>
+      </c>
+      <c r="B7" s="4">
         <f t="shared" si="3"/>
-        <v>5.375</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>5.0238095238095237</v>
+      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="G7" s="5"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="4"/>
+      <c r="Q7" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <f t="shared" si="2"/>
-        <v>327</v>
-      </c>
-      <c r="B8" s="3">
+        <v>292</v>
+      </c>
+      <c r="B8" s="4">
         <f t="shared" si="3"/>
-        <v>6.375</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+        <v>6.0238095238095237</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="Q8" s="1">
+        <f>Q6-Q7</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <f t="shared" si="2"/>
-        <v>375</v>
-      </c>
-      <c r="B9" s="3">
+        <v>334</v>
+      </c>
+      <c r="B9" s="4">
         <f t="shared" si="3"/>
-        <v>7.375</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+        <v>7.0238095238095237</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <f t="shared" si="2"/>
-        <v>423</v>
-      </c>
-      <c r="B10" s="3">
+        <v>376</v>
+      </c>
+      <c r="B10" s="4">
         <f t="shared" si="3"/>
-        <v>8.375</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
+        <v>8.0238095238095237</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f t="shared" si="2"/>
+        <v>418</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="3"/>
+        <v>9.0238095238095237</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <f t="shared" si="2"/>
+        <v>460</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="3"/>
+        <v>10.023809523809524</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Novas imagens paredes e correção explosão
</commit_message>
<xml_diff>
--- a/calc/matriz-gameboard-calc.xlsx
+++ b/calc/matriz-gameboard-calc.xlsx
@@ -8,8 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Plan1 (2)" sheetId="4" r:id="rId2"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId3"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -17,7 +18,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -27,6 +28,13 @@
     </font>
     <font>
       <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -92,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -108,6 +116,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -410,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="N9" sqref="N9:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -421,7 +438,7 @@
     <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3">
         <v>84</v>
@@ -475,7 +492,717 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>40</v>
+      </c>
+      <c r="B2" s="8" t="str">
+        <f>"createBreakableWall("&amp;$B$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(84,40)</v>
+      </c>
+      <c r="C2" s="8" t="str">
+        <f>"createBreakableWall("&amp;$C$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(126,40)</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(168,40)</v>
+      </c>
+      <c r="E2" s="8" t="str">
+        <f>"createBreakableWall("&amp;$E$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(210,40)</v>
+      </c>
+      <c r="F2" s="7" t="str">
+        <f>"createBreakableWall("&amp;$F$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(252,40)</v>
+      </c>
+      <c r="G2" s="7" t="str">
+        <f>"createBreakableWall("&amp;$G$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(294,40)</v>
+      </c>
+      <c r="H2" s="6" t="str">
+        <f>"createBreakableWall("&amp;$H$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(336,40)</v>
+      </c>
+      <c r="I2" s="8" t="str">
+        <f>"createBreakableWall("&amp;$I$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(378,40)</v>
+      </c>
+      <c r="J2" s="7" t="str">
+        <f>"createBreakableWall("&amp;$J$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(420,40)</v>
+      </c>
+      <c r="K2" s="8" t="str">
+        <f>"createBreakableWall("&amp;$K$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(462,40)</v>
+      </c>
+      <c r="L2" s="7" t="str">
+        <f>"createBreakableWall("&amp;$L$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(504,40)</v>
+      </c>
+      <c r="M2" s="8" t="str">
+        <f>"createBreakableWall("&amp;$M$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(546,40)</v>
+      </c>
+      <c r="N2" s="8" t="str">
+        <f>"createBreakableWall("&amp;$N$1&amp;","&amp;A2&amp;")"</f>
+        <v>createBreakableWall(588,40)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <f>A2+42</f>
+        <v>82</v>
+      </c>
+      <c r="B3" s="8" t="str">
+        <f>"createBreakableWall("&amp;$B$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(84,82)</v>
+      </c>
+      <c r="C3" s="6" t="str">
+        <f>"createBreakableWall("&amp;$C$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(126,82)</v>
+      </c>
+      <c r="D3" s="7" t="str">
+        <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(168,82)</v>
+      </c>
+      <c r="E3" s="6" t="str">
+        <f>"createBreakableWall("&amp;$E$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(210,82)</v>
+      </c>
+      <c r="F3" s="8" t="str">
+        <f>"createBreakableWall("&amp;$F$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(252,82)</v>
+      </c>
+      <c r="G3" s="6" t="str">
+        <f>"createBreakableWall("&amp;$G$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(294,82)</v>
+      </c>
+      <c r="H3" s="8" t="str">
+        <f>"createBreakableWall("&amp;$H$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(336,82)</v>
+      </c>
+      <c r="I3" s="6" t="str">
+        <f>"createBreakableWall("&amp;$I$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(378,82)</v>
+      </c>
+      <c r="J3" s="7" t="str">
+        <f>"createBreakableWall("&amp;$J$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(420,82)</v>
+      </c>
+      <c r="K3" s="6" t="str">
+        <f>"createBreakableWall("&amp;$K$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(462,82)</v>
+      </c>
+      <c r="L3" s="8" t="str">
+        <f>"createBreakableWall("&amp;$L$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(504,82)</v>
+      </c>
+      <c r="M3" s="6" t="str">
+        <f>"createBreakableWall("&amp;$M$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(546,82)</v>
+      </c>
+      <c r="N3" s="8" t="str">
+        <f>"createBreakableWall("&amp;$N$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(588,82)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A12" si="1">A3+42</f>
+        <v>124</v>
+      </c>
+      <c r="B4" s="7" t="str">
+        <f>"createBreakableWall("&amp;$B$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(84,124)</v>
+      </c>
+      <c r="C4" s="7" t="str">
+        <f>"createBreakableWall("&amp;$C$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(126,124)</v>
+      </c>
+      <c r="D4" s="7" t="str">
+        <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(168,124)</v>
+      </c>
+      <c r="E4" s="8" t="str">
+        <f>"createBreakableWall("&amp;$E$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(210,124)</v>
+      </c>
+      <c r="F4" s="8" t="str">
+        <f>"createBreakableWall("&amp;$F$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(252,124)</v>
+      </c>
+      <c r="G4" s="8" t="str">
+        <f>"createBreakableWall("&amp;$G$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(294,124)</v>
+      </c>
+      <c r="H4" s="7" t="str">
+        <f>"createBreakableWall("&amp;$H$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(336,124)</v>
+      </c>
+      <c r="I4" s="8" t="str">
+        <f>"createBreakableWall("&amp;$I$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(378,124)</v>
+      </c>
+      <c r="J4" s="7" t="str">
+        <f>"createBreakableWall("&amp;$J$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(420,124)</v>
+      </c>
+      <c r="K4" s="8" t="str">
+        <f>"createBreakableWall("&amp;$K$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(462,124)</v>
+      </c>
+      <c r="L4" s="8" t="str">
+        <f>"createBreakableWall("&amp;$L$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(504,124)</v>
+      </c>
+      <c r="M4" s="8" t="str">
+        <f>"createBreakableWall("&amp;$M$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(546,124)</v>
+      </c>
+      <c r="N4" s="7" t="str">
+        <f>"createBreakableWall("&amp;$N$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(588,124)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <f t="shared" si="1"/>
+        <v>166</v>
+      </c>
+      <c r="B5" s="8" t="str">
+        <f t="shared" ref="B5:B12" si="2">"createBreakableWall("&amp;$B$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(84,166)</v>
+      </c>
+      <c r="C5" s="6" t="str">
+        <f t="shared" ref="C5:C12" si="3">"createBreakableWall("&amp;$C$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(126,166)</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f t="shared" ref="D5:D12" si="4">"createBreakableWall("&amp;$D$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(168,166)</v>
+      </c>
+      <c r="E5" s="6" t="str">
+        <f t="shared" ref="E5:E12" si="5">"createBreakableWall("&amp;$E$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(210,166)</v>
+      </c>
+      <c r="F5" s="8" t="str">
+        <f t="shared" ref="F5:F12" si="6">"createBreakableWall("&amp;$F$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(252,166)</v>
+      </c>
+      <c r="G5" s="6" t="str">
+        <f t="shared" ref="G5:G12" si="7">"createBreakableWall("&amp;$G$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(294,166)</v>
+      </c>
+      <c r="H5" s="7" t="str">
+        <f t="shared" ref="H5:H12" si="8">"createBreakableWall("&amp;$H$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(336,166)</v>
+      </c>
+      <c r="I5" s="6" t="str">
+        <f t="shared" ref="I5:I12" si="9">"createBreakableWall("&amp;$I$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(378,166)</v>
+      </c>
+      <c r="J5" s="8" t="str">
+        <f t="shared" ref="J5:J12" si="10">"createBreakableWall("&amp;$J$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(420,166)</v>
+      </c>
+      <c r="K5" s="6" t="str">
+        <f t="shared" ref="K5:K12" si="11">"createBreakableWall("&amp;$K$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(462,166)</v>
+      </c>
+      <c r="L5" s="8" t="str">
+        <f t="shared" ref="L5:L12" si="12">"createBreakableWall("&amp;$L$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(504,166)</v>
+      </c>
+      <c r="M5" s="6" t="str">
+        <f t="shared" ref="M5:M12" si="13">"createBreakableWall("&amp;$M$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(546,166)</v>
+      </c>
+      <c r="N5" s="7" t="str">
+        <f t="shared" ref="N5:N12" si="14">"createBreakableWall("&amp;$N$1&amp;","&amp;A5&amp;")"</f>
+        <v>createBreakableWall(588,166)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <f t="shared" si="1"/>
+        <v>208</v>
+      </c>
+      <c r="B6" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>createBreakableWall(84,208)</v>
+      </c>
+      <c r="C6" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>createBreakableWall(126,208)</v>
+      </c>
+      <c r="D6" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>createBreakableWall(168,208)</v>
+      </c>
+      <c r="E6" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>createBreakableWall(210,208)</v>
+      </c>
+      <c r="F6" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>createBreakableWall(252,208)</v>
+      </c>
+      <c r="G6" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>createBreakableWall(294,208)</v>
+      </c>
+      <c r="H6" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>createBreakableWall(336,208)</v>
+      </c>
+      <c r="I6" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>createBreakableWall(378,208)</v>
+      </c>
+      <c r="J6" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>createBreakableWall(420,208)</v>
+      </c>
+      <c r="K6" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>createBreakableWall(462,208)</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>createBreakableWall(504,208)</v>
+      </c>
+      <c r="M6" s="8" t="str">
+        <f t="shared" si="13"/>
+        <v>createBreakableWall(546,208)</v>
+      </c>
+      <c r="N6" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>createBreakableWall(588,208)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="B7" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>createBreakableWall(84,250)</v>
+      </c>
+      <c r="C7" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>createBreakableWall(126,250)</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>createBreakableWall(168,250)</v>
+      </c>
+      <c r="E7" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>createBreakableWall(210,250)</v>
+      </c>
+      <c r="F7" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>createBreakableWall(252,250)</v>
+      </c>
+      <c r="G7" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>createBreakableWall(294,250)</v>
+      </c>
+      <c r="H7" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>createBreakableWall(336,250)</v>
+      </c>
+      <c r="I7" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>createBreakableWall(378,250)</v>
+      </c>
+      <c r="J7" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>createBreakableWall(420,250)</v>
+      </c>
+      <c r="K7" s="6" t="str">
+        <f t="shared" si="11"/>
+        <v>createBreakableWall(462,250)</v>
+      </c>
+      <c r="L7" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>createBreakableWall(504,250)</v>
+      </c>
+      <c r="M7" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>createBreakableWall(546,250)</v>
+      </c>
+      <c r="N7" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>createBreakableWall(588,250)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f t="shared" si="1"/>
+        <v>292</v>
+      </c>
+      <c r="B8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>createBreakableWall(84,292)</v>
+      </c>
+      <c r="C8" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>createBreakableWall(126,292)</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>createBreakableWall(168,292)</v>
+      </c>
+      <c r="E8" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>createBreakableWall(210,292)</v>
+      </c>
+      <c r="F8" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>createBreakableWall(252,292)</v>
+      </c>
+      <c r="G8" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>createBreakableWall(294,292)</v>
+      </c>
+      <c r="H8" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>createBreakableWall(336,292)</v>
+      </c>
+      <c r="I8" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>createBreakableWall(378,292)</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f t="shared" si="10"/>
+        <v>createBreakableWall(420,292)</v>
+      </c>
+      <c r="K8" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>createBreakableWall(462,292)</v>
+      </c>
+      <c r="L8" s="8" t="str">
+        <f t="shared" si="12"/>
+        <v>createBreakableWall(504,292)</v>
+      </c>
+      <c r="M8" s="8" t="str">
+        <f t="shared" si="13"/>
+        <v>createBreakableWall(546,292)</v>
+      </c>
+      <c r="N8" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>createBreakableWall(588,292)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <f t="shared" si="1"/>
+        <v>334</v>
+      </c>
+      <c r="B9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>createBreakableWall(84,334)</v>
+      </c>
+      <c r="C9" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>createBreakableWall(126,334)</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>createBreakableWall(168,334)</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>createBreakableWall(210,334)</v>
+      </c>
+      <c r="F9" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>createBreakableWall(252,334)</v>
+      </c>
+      <c r="G9" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>createBreakableWall(294,334)</v>
+      </c>
+      <c r="H9" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>createBreakableWall(336,334)</v>
+      </c>
+      <c r="I9" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>createBreakableWall(378,334)</v>
+      </c>
+      <c r="J9" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>createBreakableWall(420,334)</v>
+      </c>
+      <c r="K9" s="6" t="str">
+        <f t="shared" si="11"/>
+        <v>createBreakableWall(462,334)</v>
+      </c>
+      <c r="L9" s="8" t="str">
+        <f t="shared" si="12"/>
+        <v>createBreakableWall(504,334)</v>
+      </c>
+      <c r="M9" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>createBreakableWall(546,334)</v>
+      </c>
+      <c r="N9" s="7" t="str">
+        <f t="shared" si="14"/>
+        <v>createBreakableWall(588,334)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>376</v>
+      </c>
+      <c r="B10" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>createBreakableWall(84,376)</v>
+      </c>
+      <c r="C10" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>createBreakableWall(126,376)</v>
+      </c>
+      <c r="D10" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>createBreakableWall(168,376)</v>
+      </c>
+      <c r="E10" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>createBreakableWall(210,376)</v>
+      </c>
+      <c r="F10" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>createBreakableWall(252,376)</v>
+      </c>
+      <c r="G10" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>createBreakableWall(294,376)</v>
+      </c>
+      <c r="H10" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>createBreakableWall(336,376)</v>
+      </c>
+      <c r="I10" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>createBreakableWall(378,376)</v>
+      </c>
+      <c r="J10" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>createBreakableWall(420,376)</v>
+      </c>
+      <c r="K10" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>createBreakableWall(462,376)</v>
+      </c>
+      <c r="L10" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>createBreakableWall(504,376)</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f t="shared" si="13"/>
+        <v>createBreakableWall(546,376)</v>
+      </c>
+      <c r="N10" s="7" t="str">
+        <f t="shared" si="14"/>
+        <v>createBreakableWall(588,376)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f t="shared" si="1"/>
+        <v>418</v>
+      </c>
+      <c r="B11" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>createBreakableWall(84,418)</v>
+      </c>
+      <c r="C11" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>createBreakableWall(126,418)</v>
+      </c>
+      <c r="D11" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>createBreakableWall(168,418)</v>
+      </c>
+      <c r="E11" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>createBreakableWall(210,418)</v>
+      </c>
+      <c r="F11" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>createBreakableWall(252,418)</v>
+      </c>
+      <c r="G11" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>createBreakableWall(294,418)</v>
+      </c>
+      <c r="H11" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>createBreakableWall(336,418)</v>
+      </c>
+      <c r="I11" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>createBreakableWall(378,418)</v>
+      </c>
+      <c r="J11" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>createBreakableWall(420,418)</v>
+      </c>
+      <c r="K11" s="6" t="str">
+        <f t="shared" si="11"/>
+        <v>createBreakableWall(462,418)</v>
+      </c>
+      <c r="L11" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>createBreakableWall(504,418)</v>
+      </c>
+      <c r="M11" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>createBreakableWall(546,418)</v>
+      </c>
+      <c r="N11" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>createBreakableWall(588,418)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <f t="shared" si="1"/>
+        <v>460</v>
+      </c>
+      <c r="B12" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>createBreakableWall(84,460)</v>
+      </c>
+      <c r="C12" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>createBreakableWall(126,460)</v>
+      </c>
+      <c r="D12" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>createBreakableWall(168,460)</v>
+      </c>
+      <c r="E12" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>createBreakableWall(210,460)</v>
+      </c>
+      <c r="F12" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>createBreakableWall(252,460)</v>
+      </c>
+      <c r="G12" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>createBreakableWall(294,460)</v>
+      </c>
+      <c r="H12" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>createBreakableWall(336,460)</v>
+      </c>
+      <c r="I12" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>createBreakableWall(378,460)</v>
+      </c>
+      <c r="J12" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>createBreakableWall(420,460)</v>
+      </c>
+      <c r="K12" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v>createBreakableWall(462,460)</v>
+      </c>
+      <c r="L12" s="8" t="str">
+        <f t="shared" si="12"/>
+        <v>createBreakableWall(504,460)</v>
+      </c>
+      <c r="M12" s="8" t="str">
+        <f t="shared" si="13"/>
+        <v>createBreakableWall(546,460)</v>
+      </c>
+      <c r="N12" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>createBreakableWall(588,460)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="8.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3">
+        <v>84</v>
+      </c>
+      <c r="C1" s="3">
+        <f>B1+42</f>
+        <v>126</v>
+      </c>
+      <c r="D1" s="3">
+        <f t="shared" ref="D1:N1" si="0">C1+42</f>
+        <v>168</v>
+      </c>
+      <c r="E1" s="3">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="F1" s="3">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="G1" s="3">
+        <f t="shared" si="0"/>
+        <v>294</v>
+      </c>
+      <c r="H1" s="3">
+        <f t="shared" si="0"/>
+        <v>336</v>
+      </c>
+      <c r="I1" s="3">
+        <f t="shared" si="0"/>
+        <v>378</v>
+      </c>
+      <c r="J1" s="3">
+        <f t="shared" si="0"/>
+        <v>420</v>
+      </c>
+      <c r="K1" s="3">
+        <f t="shared" si="0"/>
+        <v>462</v>
+      </c>
+      <c r="L1" s="3">
+        <f t="shared" si="0"/>
+        <v>504</v>
+      </c>
+      <c r="M1" s="3">
+        <f t="shared" si="0"/>
+        <v>546</v>
+      </c>
+      <c r="N1" s="3">
+        <f t="shared" si="0"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>40</v>
       </c>
@@ -488,18 +1215,18 @@
         <v>1</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="C2:N2" si="1">(D1-84)/42</f>
+        <f t="shared" ref="D2:N2" si="1">(D1-84)/42</f>
         <v>2</v>
       </c>
       <c r="E2" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -511,7 +1238,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -519,7 +1246,7 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -532,7 +1259,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>A2+42</f>
         <v>82</v>
@@ -541,56 +1268,48 @@
         <f>(A3-39)/42</f>
         <v>1.0238095238095237</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="4"/>
-      <c r="Q3" s="1">
-        <v>81</v>
-      </c>
-      <c r="R3" s="1">
-        <f>Q3-84</f>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="str">
+        <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A3&amp;")"</f>
+        <v>createBreakableWall(168,82)</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A12" si="2">A3+42</f>
         <v>124</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <f t="shared" ref="B4:B12" si="3">(A4-39)/42</f>
         <v>2.0238095238095237</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="Q4" s="1">
-        <v>33</v>
-      </c>
-      <c r="R4" s="1">
-        <f>Q4-8</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="str">
+        <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A4&amp;")"</f>
+        <v>createBreakableWall(168,124)</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="2"/>
         <v>166</v>
@@ -599,20 +1318,20 @@
         <f t="shared" si="3"/>
         <v>3.0238095238095237</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="4"/>
-    </row>
-    <row r="6" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="6"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="2"/>
         <v>208</v>
@@ -621,23 +1340,23 @@
         <f t="shared" si="3"/>
         <v>4.0238095238095237</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="Q6" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7" t="str">
+        <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A6&amp;")"</f>
+        <v>createBreakableWall(168,208)</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+    </row>
+    <row r="7" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="2"/>
         <v>250</v>
@@ -646,23 +1365,20 @@
         <f t="shared" si="3"/>
         <v>5.0238095238095237</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="4"/>
-      <c r="Q7" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="6"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="8"/>
+    </row>
+    <row r="8" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="2"/>
         <v>292</v>
@@ -671,24 +1387,20 @@
         <f t="shared" si="3"/>
         <v>6.0238095238095237</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="Q8" s="1">
-        <f>Q6-Q7</f>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="2"/>
         <v>334</v>
@@ -697,20 +1409,20 @@
         <f t="shared" si="3"/>
         <v>7.0238095238095237</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="4"/>
-    </row>
-    <row r="10" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="6"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="2"/>
         <v>376</v>
@@ -719,20 +1431,23 @@
         <f t="shared" si="3"/>
         <v>8.0238095238095237</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="6"/>
+      <c r="D10" s="7" t="str">
+        <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A10&amp;")"</f>
+        <v>createBreakableWall(168,376)</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="2"/>
         <v>418</v>
@@ -741,20 +1456,23 @@
         <f t="shared" si="3"/>
         <v>9.0238095238095237</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="6"/>
+      <c r="D11" s="7" t="str">
+        <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A11&amp;")"</f>
+        <v>createBreakableWall(168,418)</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="2"/>
         <v>460</v>
@@ -779,18 +1497,6 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
@@ -804,4 +1510,16 @@
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Animação movimentação a direita
</commit_message>
<xml_diff>
--- a/calc/matriz-gameboard-calc.xlsx
+++ b/calc/matriz-gameboard-calc.xlsx
@@ -427,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9:N10"/>
+      <selection activeCell="R6" sqref="R6:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -438,7 +438,7 @@
     <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3">
         <v>84</v>
@@ -492,7 +492,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>40</v>
       </c>
@@ -548,8 +548,18 @@
         <f>"createBreakableWall("&amp;$N$1&amp;","&amp;A2&amp;")"</f>
         <v>createBreakableWall(588,40)</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="1">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>42</v>
+      </c>
+      <c r="R2" s="1">
+        <f>P2+Q2</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>A2+42</f>
         <v>82</v>
@@ -606,8 +616,19 @@
         <f>"createBreakableWall("&amp;$N$1&amp;","&amp;A3&amp;")"</f>
         <v>createBreakableWall(588,82)</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="1">
+        <f>P2+Q3</f>
+        <v>91</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>7</v>
+      </c>
+      <c r="R3" s="1">
+        <f>Q3</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A12" si="1">A3+42</f>
         <v>124</v>
@@ -664,8 +685,19 @@
         <f>"createBreakableWall("&amp;$N$1&amp;","&amp;A4&amp;")"</f>
         <v>createBreakableWall(588,124)</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="1">
+        <f>P3+Q4</f>
+        <v>98</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>7</v>
+      </c>
+      <c r="R4" s="1">
+        <f>R3+Q4</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="1"/>
         <v>166</v>
@@ -722,8 +754,19 @@
         <f t="shared" ref="N5:N12" si="14">"createBreakableWall("&amp;$N$1&amp;","&amp;A5&amp;")"</f>
         <v>createBreakableWall(588,166)</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="1">
+        <f>P4+Q5</f>
+        <v>105</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>7</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="shared" ref="R5:R8" si="15">R4+Q5</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="1"/>
         <v>208</v>
@@ -780,8 +823,19 @@
         <f t="shared" si="14"/>
         <v>createBreakableWall(588,208)</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="1">
+        <f>P5+Q6</f>
+        <v>112</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>7</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" si="15"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="1"/>
         <v>250</v>
@@ -838,8 +892,19 @@
         <f t="shared" si="14"/>
         <v>createBreakableWall(588,250)</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="1">
+        <f>P6+Q7</f>
+        <v>119</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>7</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="15"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="1"/>
         <v>292</v>
@@ -896,8 +961,15 @@
         <f t="shared" si="14"/>
         <v>createBreakableWall(588,292)</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="1">
+        <v>7</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="15"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="1"/>
         <v>334</v>
@@ -954,8 +1026,12 @@
         <f t="shared" si="14"/>
         <v>createBreakableWall(588,334)</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="1">
+        <f>SUM(Q3:Q8)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="1"/>
         <v>376</v>
@@ -1013,7 +1089,7 @@
         <v>createBreakableWall(588,376)</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="1"/>
         <v>418</v>
@@ -1071,7 +1147,7 @@
         <v>createBreakableWall(588,418)</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="1"/>
         <v>460</v>

</xml_diff>

<commit_message>
Testes da sequencia de explosão
</commit_message>
<xml_diff>
--- a/calc/matriz-gameboard-calc.xlsx
+++ b/calc/matriz-gameboard-calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6:R8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1213,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1224,7 @@
     <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3">
         <v>84</v>
@@ -1278,7 +1278,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>40</v>
       </c>
@@ -1334,8 +1334,26 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>43</v>
+      </c>
+      <c r="R2" s="1">
+        <f>Q2+43</f>
+        <v>86</v>
+      </c>
+      <c r="S2" s="1">
+        <f t="shared" ref="S2:T2" si="2">R2+43</f>
+        <v>129</v>
+      </c>
+      <c r="T2" s="1">
+        <f t="shared" si="2"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>A2+42</f>
         <v>82</v>
@@ -1360,13 +1378,13 @@
       <c r="M3" s="6"/>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A12" si="2">A3+42</f>
+        <f t="shared" ref="A4:A12" si="3">A3+42</f>
         <v>124</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B12" si="3">(A4-39)/42</f>
+        <f t="shared" ref="B4:B12" si="4">(A4-39)/42</f>
         <v>2.0238095238095237</v>
       </c>
       <c r="C4" s="7"/>
@@ -1385,13 +1403,13 @@
       <c r="M4" s="8"/>
       <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>166</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.0238095238095237</v>
       </c>
       <c r="C5" s="6"/>
@@ -1407,13 +1425,13 @@
       <c r="M5" s="6"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208</v>
       </c>
       <c r="B6" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.0238095238095237</v>
       </c>
       <c r="C6" s="7"/>
@@ -1432,13 +1450,13 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>250</v>
       </c>
       <c r="B7" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.0238095238095237</v>
       </c>
       <c r="C7" s="6"/>
@@ -1454,13 +1472,13 @@
       <c r="M7" s="6"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>292</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.0238095238095237</v>
       </c>
       <c r="C8" s="8"/>
@@ -1476,13 +1494,13 @@
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>334</v>
       </c>
       <c r="B9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.0238095238095237</v>
       </c>
       <c r="C9" s="6"/>
@@ -1498,13 +1516,13 @@
       <c r="M9" s="6"/>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>376</v>
       </c>
       <c r="B10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.0238095238095237</v>
       </c>
       <c r="C10" s="6"/>
@@ -1523,13 +1541,13 @@
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>418</v>
       </c>
       <c r="B11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.0238095238095237</v>
       </c>
       <c r="C11" s="6"/>
@@ -1548,13 +1566,13 @@
       <c r="M11" s="6"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>460</v>
       </c>
       <c r="B12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.023809523809524</v>
       </c>
       <c r="C12" s="5"/>

</xml_diff>

<commit_message>
Correção movimentação errada bomberman
</commit_message>
<xml_diff>
--- a/calc/matriz-gameboard-calc.xlsx
+++ b/calc/matriz-gameboard-calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,9 +16,20 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>positionLeft</t>
+  </si>
+  <si>
+    <t>positionTop</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -35,6 +46,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -100,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -125,6 +143,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1213,15 +1237,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1234,11 +1260,11 @@
         <v>126</v>
       </c>
       <c r="D1" s="3">
-        <f t="shared" ref="D1:N1" si="0">C1+42</f>
+        <f>C1+42</f>
         <v>168</v>
       </c>
       <c r="E1" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D1:N1" si="0">D1+42</f>
         <v>210</v>
       </c>
       <c r="F1" s="3">
@@ -1280,7 +1306,7 @@
     </row>
     <row r="2" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4">
         <f>(B1-84)/42</f>
@@ -1291,11 +1317,11 @@
         <v>1</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:N2" si="1">(D1-84)/42</f>
+        <f>(D1-84)/42</f>
         <v>2</v>
       </c>
       <c r="E2" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E2:N2" si="1">(E1-84)/42</f>
         <v>3</v>
       </c>
       <c r="F2" s="2">
@@ -1356,16 +1382,16 @@
     <row r="3" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>A2+42</f>
-        <v>82</v>
-      </c>
-      <c r="B3" s="4">
-        <f>(A3-39)/42</f>
-        <v>1.0238095238095237</v>
+        <v>50</v>
+      </c>
+      <c r="B3" s="10">
+        <f>(A3-8)/42</f>
+        <v>1</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="str">
         <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A3&amp;")"</f>
-        <v>createBreakableWall(168,82)</v>
+        <v>createBreakableWall(168,50)</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="8"/>
@@ -1381,16 +1407,16 @@
     <row r="4" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A12" si="3">A3+42</f>
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B12" si="4">(A4-39)/42</f>
-        <v>2.0238095238095237</v>
+        <f>(A4-8)/42</f>
+        <v>2</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="str">
         <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A4&amp;")"</f>
-        <v>createBreakableWall(168,124)</v>
+        <v>createBreakableWall(168,92)</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -1406,11 +1432,11 @@
     <row r="5" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="3"/>
-        <v>166</v>
-      </c>
-      <c r="B5" s="4">
-        <f t="shared" si="4"/>
-        <v>3.0238095238095237</v>
+        <v>134</v>
+      </c>
+      <c r="B5" s="10">
+        <f>(A5-8)/42</f>
+        <v>3</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="8"/>
@@ -1428,16 +1454,16 @@
     <row r="6" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="3"/>
-        <v>208</v>
-      </c>
-      <c r="B6" s="4">
-        <f t="shared" si="4"/>
-        <v>4.0238095238095237</v>
+        <v>176</v>
+      </c>
+      <c r="B6" s="10">
+        <f>(A6-8)/42</f>
+        <v>4</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="str">
         <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A6&amp;")"</f>
-        <v>createBreakableWall(168,208)</v>
+        <v>createBreakableWall(168,176)</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -1453,11 +1479,11 @@
     <row r="7" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="3"/>
-        <v>250</v>
-      </c>
-      <c r="B7" s="4">
-        <f t="shared" si="4"/>
-        <v>5.0238095238095237</v>
+        <v>218</v>
+      </c>
+      <c r="B7" s="10">
+        <f t="shared" ref="B7:B12" si="4">(A7-8)/42</f>
+        <v>5</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="8"/>
@@ -1475,11 +1501,11 @@
     <row r="8" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="3"/>
-        <v>292</v>
-      </c>
-      <c r="B8" s="4">
+        <v>260</v>
+      </c>
+      <c r="B8" s="10">
         <f t="shared" si="4"/>
-        <v>6.0238095238095237</v>
+        <v>6</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1497,11 +1523,11 @@
     <row r="9" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="3"/>
-        <v>334</v>
-      </c>
-      <c r="B9" s="4">
+        <v>302</v>
+      </c>
+      <c r="B9" s="10">
         <f t="shared" si="4"/>
-        <v>7.0238095238095237</v>
+        <v>7</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="8"/>
@@ -1519,16 +1545,16 @@
     <row r="10" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="3"/>
-        <v>376</v>
-      </c>
-      <c r="B10" s="4">
+        <v>344</v>
+      </c>
+      <c r="B10" s="10">
         <f t="shared" si="4"/>
-        <v>8.0238095238095237</v>
+        <v>8</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="7" t="str">
         <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A10&amp;")"</f>
-        <v>createBreakableWall(168,376)</v>
+        <v>createBreakableWall(168,344)</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -1544,16 +1570,16 @@
     <row r="11" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="3"/>
-        <v>418</v>
-      </c>
-      <c r="B11" s="4">
-        <f t="shared" si="4"/>
-        <v>9.0238095238095237</v>
+        <v>386</v>
+      </c>
+      <c r="B11" s="10">
+        <f>(A11-8)/42</f>
+        <v>9</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="7" t="str">
         <f>"createBreakableWall("&amp;$D$1&amp;","&amp;A11&amp;")"</f>
-        <v>createBreakableWall(168,418)</v>
+        <v>createBreakableWall(168,386)</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="8"/>
@@ -1569,11 +1595,11 @@
     <row r="12" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="3"/>
-        <v>460</v>
-      </c>
-      <c r="B12" s="4">
+        <v>428</v>
+      </c>
+      <c r="B12" s="10">
         <f t="shared" si="4"/>
-        <v>10.023809523809524</v>
+        <v>10</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4"/>
@@ -1588,7 +1614,130 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
+    <row r="15" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <f>(D16-84)/42</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <f>(E16-84)/42</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" ref="F15:J15" si="5">(F16-84)/42</f>
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="5"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="5"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="K15" s="1">
+        <f>(K16-84)/42</f>
+        <v>2.9523809523809526</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" ref="L15" si="6">(L16-84)/42</f>
+        <v>2.9761904761904763</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" ref="M15" si="7">(M16-84)/42</f>
+        <v>3</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" ref="N15:O15" si="8">(N16-84)/42</f>
+        <v>3.0238095238095237</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="8"/>
+        <v>3.0714285714285716</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="1">
+        <v>84</v>
+      </c>
+      <c r="E16" s="1">
+        <v>126</v>
+      </c>
+      <c r="F16" s="1">
+        <v>168</v>
+      </c>
+      <c r="G16" s="1">
+        <v>112</v>
+      </c>
+      <c r="H16" s="1">
+        <v>140</v>
+      </c>
+      <c r="I16" s="1">
+        <v>168</v>
+      </c>
+      <c r="J16" s="1">
+        <v>182</v>
+      </c>
+      <c r="K16" s="1">
+        <v>208</v>
+      </c>
+      <c r="L16" s="1">
+        <v>209</v>
+      </c>
+      <c r="M16" s="1">
+        <v>210</v>
+      </c>
+      <c r="N16" s="1">
+        <v>211</v>
+      </c>
+      <c r="O16" s="1">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="1">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1">
+        <v>8</v>
+      </c>
+      <c r="G17" s="1">
+        <v>8</v>
+      </c>
+      <c r="H17" s="1">
+        <v>8</v>
+      </c>
+      <c r="I17" s="1">
+        <v>8</v>
+      </c>
+      <c r="J17" s="1">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Automatização da criação de paredes quebraveis
</commit_message>
<xml_diff>
--- a/calc/matriz-gameboard-calc.xlsx
+++ b/calc/matriz-gameboard-calc.xlsx
@@ -9,20 +9,129 @@
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan1 (2)" sheetId="4" r:id="rId2"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId3"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId4"/>
+    <sheet name="Plan1 (3)" sheetId="5" r:id="rId3"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId4"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>positionLeft</t>
   </si>
   <si>
     <t>positionTop</t>
+  </si>
+  <si>
+    <t>126;376',</t>
+  </si>
+  <si>
+    <t>210;82',</t>
+  </si>
+  <si>
+    <t>294;82',</t>
+  </si>
+  <si>
+    <t>336;376',</t>
+  </si>
+  <si>
+    <t>378;82',</t>
+  </si>
+  <si>
+    <t>462;82',</t>
+  </si>
+  <si>
+    <t>504;418',</t>
+  </si>
+  <si>
+    <t>546;82',</t>
+  </si>
+  <si>
+    <t>126;82',</t>
+  </si>
+  <si>
+    <t>210;166',</t>
+  </si>
+  <si>
+    <t>294;166',</t>
+  </si>
+  <si>
+    <t>336;40',</t>
+  </si>
+  <si>
+    <t>378;166',</t>
+  </si>
+  <si>
+    <t>462;166',</t>
+  </si>
+  <si>
+    <t>546;166',</t>
+  </si>
+  <si>
+    <t>126;166',</t>
+  </si>
+  <si>
+    <t>210;250',</t>
+  </si>
+  <si>
+    <t>294;250',</t>
+  </si>
+  <si>
+    <t>378;250',</t>
+  </si>
+  <si>
+    <t>462;250',</t>
+  </si>
+  <si>
+    <t>546;250',</t>
+  </si>
+  <si>
+    <t>126;250',</t>
+  </si>
+  <si>
+    <t>210;334',</t>
+  </si>
+  <si>
+    <t>294;334',</t>
+  </si>
+  <si>
+    <t>378;334',</t>
+  </si>
+  <si>
+    <t>462;334',</t>
+  </si>
+  <si>
+    <t>546;334',</t>
+  </si>
+  <si>
+    <t>126;418',</t>
+  </si>
+  <si>
+    <t>126;460',</t>
+  </si>
+  <si>
+    <t>294;292',</t>
+  </si>
+  <si>
+    <t>126;334',</t>
+  </si>
+  <si>
+    <t>210;418',</t>
+  </si>
+  <si>
+    <t>294;418',</t>
+  </si>
+  <si>
+    <t>378;418',</t>
+  </si>
+  <si>
+    <t>462;418',</t>
+  </si>
+  <si>
+    <t>546;418',</t>
   </si>
 </sst>
 </file>
@@ -118,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -144,17 +253,77 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE26B0A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE26B0A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE26B0A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE26B0A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE26B0A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE26B0A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE26B0A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -454,7 +623,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1433,7 @@
         <v>168</v>
       </c>
       <c r="E1" s="3">
-        <f t="shared" ref="D1:N1" si="0">D1+42</f>
+        <f t="shared" ref="E1:N1" si="0">D1+42</f>
         <v>210</v>
       </c>
       <c r="F1" s="3">
@@ -1384,7 +1553,7 @@
         <f>A2+42</f>
         <v>50</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <f>(A3-8)/42</f>
         <v>1</v>
       </c>
@@ -1434,7 +1603,7 @@
         <f t="shared" si="3"/>
         <v>134</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <f>(A5-8)/42</f>
         <v>3</v>
       </c>
@@ -1456,7 +1625,7 @@
         <f t="shared" si="3"/>
         <v>176</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <f>(A6-8)/42</f>
         <v>4</v>
       </c>
@@ -1481,7 +1650,7 @@
         <f t="shared" si="3"/>
         <v>218</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <f t="shared" ref="B7:B12" si="4">(A7-8)/42</f>
         <v>5</v>
       </c>
@@ -1503,7 +1672,7 @@
         <f t="shared" si="3"/>
         <v>260</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
@@ -1525,7 +1694,7 @@
         <f t="shared" si="3"/>
         <v>302</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
@@ -1547,7 +1716,7 @@
         <f t="shared" si="3"/>
         <v>344</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
@@ -1572,7 +1741,7 @@
         <f t="shared" si="3"/>
         <v>386</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <f>(A11-8)/42</f>
         <v>9</v>
       </c>
@@ -1597,7 +1766,7 @@
         <f t="shared" si="3"/>
         <v>428</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
@@ -1665,10 +1834,10 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="1">
         <v>84</v>
       </c>
@@ -1707,10 +1876,10 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="1">
         <v>8</v>
       </c>
@@ -1745,17 +1914,239 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection sqref="A1:AJ1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="8.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:L13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>40</v>
+      </c>
+      <c r="C13">
+        <v>82</v>
+      </c>
+      <c r="D13">
+        <v>124</v>
+      </c>
+      <c r="E13">
+        <v>166</v>
+      </c>
+      <c r="F13">
+        <v>208</v>
+      </c>
+      <c r="G13">
+        <v>250</v>
+      </c>
+      <c r="H13">
+        <v>292</v>
+      </c>
+      <c r="I13">
+        <v>334</v>
+      </c>
+      <c r="J13">
+        <v>376</v>
+      </c>
+      <c r="K13">
+        <v>418</v>
+      </c>
+      <c r="L13">
+        <v>460</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>